<commit_message>
team template and rosters
</commit_message>
<xml_diff>
--- a/teams-and-rosters/CS320-Sp24-101-roster.xlsx
+++ b/teams-and-rosters/CS320-Sp24-101-roster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\teams-and-rosters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBA959F-6A32-4D78-833F-AFD98CB0DFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27517BA8-D950-4B1A-AB04-4AB3CD4ECA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="667" windowWidth="26355" windowHeight="14858" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1289,6 +1289,8 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="155" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>